<commit_message>
Added excel read and write methods
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/DomainsJourneyMockData.xlsx
+++ b/src/test/resources/testData/DomainsJourneyMockData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc88eea5f909387f/Desktop/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="275">
   <si>
     <t>CustomerID (required)</t>
   </si>
@@ -857,12 +857,16 @@
   </si>
   <si>
     <t>Actual actions</t>
+  </si>
+  <si>
+    <t>actaul response</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1307,49 +1311,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="43" customWidth="1"/>
-    <col min="2" max="2" width="33.5234375" customWidth="1"/>
-    <col min="3" max="3" width="27.1015625" customWidth="1"/>
-    <col min="4" max="4" width="31.5234375" customWidth="1"/>
-    <col min="5" max="5" width="20.7890625" customWidth="1"/>
-    <col min="6" max="6" width="20.1015625" customWidth="1"/>
-    <col min="14" max="15" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.3125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="23" max="57" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="17.3125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="11.20703125" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="17.3125" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="12.3671875" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="17.3125" bestFit="1" customWidth="1"/>
-    <col min="109" max="110" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="113" max="114" width="17.3125" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="17.3125" bestFit="1" customWidth="1"/>
-    <col min="120" max="121" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="123" max="124" width="17.3125" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="132" max="179" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="185" max="185" width="13.578125" bestFit="1" customWidth="1"/>
-    <col min="189" max="190" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="196" max="196" width="10.05078125" bestFit="1" customWidth="1"/>
-    <col min="199" max="199" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="200" max="200" width="16.05078125" customWidth="1"/>
-    <col min="201" max="201" width="18.5234375" customWidth="1"/>
-    <col min="202" max="202" width="14.15625" customWidth="1"/>
-    <col min="203" max="203" width="17.62890625" customWidth="1"/>
-    <col min="204" max="204" width="14.15625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="43.0"/>
+    <col min="2" max="2" customWidth="true" width="33.5234375"/>
+    <col min="3" max="3" customWidth="true" width="27.1015625"/>
+    <col min="4" max="4" customWidth="true" width="31.5234375"/>
+    <col min="5" max="5" customWidth="true" width="20.7890625"/>
+    <col min="6" max="6" customWidth="true" width="20.1015625"/>
+    <col min="14" max="15" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="17.3125"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="23" max="57" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="64" max="64" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="69" max="69" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="72" max="72" bestFit="true" customWidth="true" width="17.3125"/>
+    <col min="73" max="73" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="76" max="76" bestFit="true" customWidth="true" width="11.20703125"/>
+    <col min="82" max="82" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="85" max="85" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="88" max="88" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="95" max="95" bestFit="true" customWidth="true" width="17.3125"/>
+    <col min="96" max="96" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="99" max="99" bestFit="true" customWidth="true" width="12.3671875"/>
+    <col min="105" max="105" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="108" max="108" bestFit="true" customWidth="true" width="17.3125"/>
+    <col min="109" max="110" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="113" max="114" bestFit="true" customWidth="true" width="17.3125"/>
+    <col min="115" max="115" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="117" max="117" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="119" max="119" bestFit="true" customWidth="true" width="17.3125"/>
+    <col min="120" max="121" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="123" max="124" bestFit="true" customWidth="true" width="17.3125"/>
+    <col min="125" max="125" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="127" max="127" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="129" max="129" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="132" max="179" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="185" max="185" bestFit="true" customWidth="true" width="13.578125"/>
+    <col min="189" max="190" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="196" max="196" bestFit="true" customWidth="true" width="10.05078125"/>
+    <col min="199" max="199" bestFit="true" customWidth="true" width="8.89453125"/>
+    <col min="200" max="200" customWidth="true" width="16.05078125"/>
+    <col min="201" max="201" customWidth="true" width="18.5234375"/>
+    <col min="202" max="202" customWidth="true" width="14.15625"/>
+    <col min="203" max="203" customWidth="true" width="17.62890625"/>
+    <col min="204" max="204" customWidth="true" width="14.15625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:205" ht="15.6" x14ac:dyDescent="0.6">
@@ -1554,6 +1558,9 @@
       <c r="GQ1" s="2"/>
       <c r="GR1" s="2"/>
       <c r="GS1" s="2"/>
+      <c r="GT1" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="2" spans="1:205" ht="15.3" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="3" t="s">
@@ -2160,7 +2167,7 @@
         <v>268</v>
       </c>
       <c r="GT2" s="9" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="GU2" s="9" t="s">
         <v>272</v>
@@ -2626,6 +2633,9 @@
       <c r="GS3" s="7" t="s">
         <v>271</v>
       </c>
+      <c r="GT3" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="4" spans="1:205" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
@@ -3147,6 +3157,9 @@
       </c>
       <c r="GR4" s="5"/>
       <c r="GS4" s="7"/>
+      <c r="GT4" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="5" spans="1:205" ht="15.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
@@ -3636,9 +3649,20 @@
       </c>
       <c r="GR5" s="5"/>
       <c r="GS5" s="5"/>
+      <c r="GT5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="GT6" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="7" spans="1:205" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B7" s="1"/>
+      <c r="GT7" t="s">
+        <v>274</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>